<commit_message>
Revisio documentació - ultims canvis api
</commit_message>
<xml_diff>
--- a/documentacio/Planifiació_GANTT.xlsx
+++ b/documentacio/Planifiació_GANTT.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr filterPrivacy="1" codeName="AquestLlibreDeTreball"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{160866E4-9E50-4118-83BD-B652364C863E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ABAD28B-108B-4718-A21A-C3D3DE523E8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="472" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="472" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PROJECTE" sheetId="11" r:id="rId1"/>
@@ -19,10 +19,21 @@
     <definedName name="task_start" localSheetId="0">PROJECTE!$E1</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">PROJECTE!$4:$6</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1165,58 +1176,58 @@
     </xf>
   </cellXfs>
   <cellStyles count="54">
-    <cellStyle name="20% - Èmfasi1" xfId="31" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Èmfasi2" xfId="35" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Èmfasi3" xfId="39" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Èmfasi4" xfId="43" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Èmfasi5" xfId="47" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Èmfasi6" xfId="51" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Èmfasi1" xfId="32" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Èmfasi2" xfId="36" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Èmfasi3" xfId="40" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Èmfasi4" xfId="44" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Èmfasi5" xfId="48" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Èmfasi6" xfId="52" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Èmfasi1" xfId="33" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Èmfasi2" xfId="37" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Èmfasi3" xfId="41" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Èmfasi4" xfId="45" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Èmfasi5" xfId="49" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Èmfasi6" xfId="53" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Bé" xfId="18" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Càlcul" xfId="23" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Cel·la de comprovació" xfId="25" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Cel·la enllaçada" xfId="24" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Coma" xfId="4" builtinId="3" customBuiltin="1"/>
-    <cellStyle name="Èmfasi1" xfId="30" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Èmfasi2" xfId="34" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Èmfasi3" xfId="38" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Èmfasi4" xfId="42" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Èmfasi5" xfId="46" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Èmfasi6" xfId="50" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Enllaç" xfId="1" builtinId="8" customBuiltin="1"/>
-    <cellStyle name="Enllaç visitat" xfId="13" builtinId="9" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis1" xfId="31" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis2" xfId="35" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis3" xfId="39" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis4" xfId="43" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis5" xfId="47" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis6" xfId="51" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis1" xfId="32" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis2" xfId="36" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis3" xfId="40" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis4" xfId="44" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis5" xfId="48" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis6" xfId="52" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis1" xfId="33" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis2" xfId="37" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis3" xfId="41" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis4" xfId="45" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis5" xfId="49" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis6" xfId="53" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Bueno" xfId="18" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Cálculo" xfId="23" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Celda de comprobación" xfId="25" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Celda vinculada" xfId="24" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Encabezado 1" xfId="6" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Encabezado 4" xfId="17" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Énfasis1" xfId="30" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Énfasis2" xfId="34" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Énfasis3" xfId="38" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Énfasis4" xfId="42" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Énfasis5" xfId="46" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Énfasis6" xfId="50" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Entrada" xfId="21" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Fecha" xfId="10" xr:uid="{229918B6-DD13-4F5A-97B9-305F7E002AA3}"/>
-    <cellStyle name="Incorrecte" xfId="19" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8" customBuiltin="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="13" builtinId="9" customBuiltin="1"/>
+    <cellStyle name="Incorrecto" xfId="19" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Inicio del proyecto" xfId="9" xr:uid="{8EB8A09A-C31C-40A3-B2C1-9449520178B8}"/>
-    <cellStyle name="Milers [0]" xfId="14" builtinId="6" customBuiltin="1"/>
+    <cellStyle name="Millares" xfId="4" builtinId="3" customBuiltin="1"/>
+    <cellStyle name="Millares [0]" xfId="14" builtinId="6" customBuiltin="1"/>
     <cellStyle name="Moneda" xfId="15" builtinId="4" customBuiltin="1"/>
     <cellStyle name="Moneda [0]" xfId="16" builtinId="7" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="20" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Nombre" xfId="11" xr:uid="{B2D3C1EE-6B41-4801-AAFC-C2274E49E503}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Nota" xfId="27" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Percentatge" xfId="2" builtinId="5" customBuiltin="1"/>
-    <cellStyle name="Resultat" xfId="22" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Notas" xfId="27" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Porcentaje" xfId="2" builtinId="5" customBuiltin="1"/>
+    <cellStyle name="Salida" xfId="22" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Tarea" xfId="12" xr:uid="{6391D789-272B-4DD2-9BF3-2CDCF610FA41}"/>
-    <cellStyle name="Text d'advertiment" xfId="26" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Text explicatiu" xfId="28" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Títol" xfId="5" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Títol 1" xfId="6" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Títol 2" xfId="7" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Títol 3" xfId="8" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Títol 4" xfId="17" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Texto de advertencia" xfId="26" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Texto explicativo" xfId="28" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Título" xfId="5" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Título 2" xfId="7" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Título 3" xfId="8" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="29" builtinId="25" customBuiltin="1"/>
     <cellStyle name="zTextoOculto" xfId="3" xr:uid="{26E66EE6-E33F-4D77-BAE4-0FB4F5BBF673}"/>
   </cellStyles>
@@ -1770,25 +1781,25 @@
   </sheetPr>
   <dimension ref="A1:EK30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E30" sqref="E30"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AR12" sqref="AR12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="25" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" customWidth="1"/>
-    <col min="7" max="7" width="2.85546875" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="5.28515625" hidden="1" customWidth="1"/>
-    <col min="9" max="141" width="2.28515625" customWidth="1"/>
+    <col min="1" max="1" width="2.7265625" style="25" customWidth="1"/>
+    <col min="2" max="2" width="29.7265625" customWidth="1"/>
+    <col min="3" max="3" width="30.7265625" customWidth="1"/>
+    <col min="4" max="4" width="10.7265625" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="10.453125" customWidth="1"/>
+    <col min="7" max="7" width="2.81640625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="5.26953125" hidden="1" customWidth="1"/>
+    <col min="9" max="141" width="2.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:141" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:141" ht="30" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
@@ -1802,7 +1813,7 @@
       <c r="H1" s="2"/>
       <c r="I1" s="44"/>
     </row>
-    <row r="2" spans="1:141" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:141" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
@@ -1811,7 +1822,7 @@
       </c>
       <c r="I2" s="45"/>
     </row>
-    <row r="3" spans="1:141" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:141" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="25" t="s">
         <v>2</v>
       </c>
@@ -1827,7 +1838,7 @@
       </c>
       <c r="F3" s="73"/>
     </row>
-    <row r="4" spans="1:141" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:141" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="26" t="s">
         <v>3</v>
       </c>
@@ -2030,7 +2041,7 @@
       <c r="EJ4" s="71"/>
       <c r="EK4" s="72"/>
     </row>
-    <row r="5" spans="1:141" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:141" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="26" t="s">
         <v>4</v>
       </c>
@@ -2573,7 +2584,7 @@
         <v>45837</v>
       </c>
     </row>
-    <row r="6" spans="1:141" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:141" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="26" t="s">
         <v>5</v>
       </c>
@@ -2728,7 +2739,7 @@
       <c r="EJ6" s="8"/>
       <c r="EK6" s="8"/>
     </row>
-    <row r="7" spans="1:141" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:141" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="25" t="s">
         <v>6</v>
       </c>
@@ -2795,7 +2806,7 @@
       <c r="BK7" s="22"/>
       <c r="BL7" s="22"/>
     </row>
-    <row r="8" spans="1:141" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:141" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="26" t="s">
         <v>7</v>
       </c>
@@ -2805,7 +2816,7 @@
       <c r="C8" s="31"/>
       <c r="D8" s="11">
         <f>AVERAGE(D9:D12)</f>
-        <v>0.8125</v>
+        <v>1</v>
       </c>
       <c r="E8" s="46">
         <v>45704</v>
@@ -2952,7 +2963,7 @@
       <c r="EJ8" s="22"/>
       <c r="EK8" s="22"/>
     </row>
-    <row r="9" spans="1:141" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:141" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="26" t="s">
         <v>8</v>
       </c>
@@ -3109,7 +3120,7 @@
       <c r="EJ9" s="22"/>
       <c r="EK9" s="22"/>
     </row>
-    <row r="10" spans="1:141" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:141" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="26" t="s">
         <v>9</v>
       </c>
@@ -3266,7 +3277,7 @@
       <c r="EJ10" s="22"/>
       <c r="EK10" s="22"/>
     </row>
-    <row r="11" spans="1:141" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:141" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="25"/>
       <c r="B11" s="39" t="s">
         <v>21</v>
@@ -3421,14 +3432,14 @@
       <c r="EJ11" s="22"/>
       <c r="EK11" s="22"/>
     </row>
-    <row r="12" spans="1:141" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:141" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="25"/>
       <c r="B12" s="39" t="s">
         <v>22</v>
       </c>
       <c r="C12" s="32"/>
       <c r="D12" s="12">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="E12" s="48">
         <f>Inicio_del_proyecto</f>
@@ -3576,7 +3587,7 @@
       <c r="EJ12" s="22"/>
       <c r="EK12" s="22"/>
     </row>
-    <row r="13" spans="1:141" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:141" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="26" t="s">
         <v>10</v>
       </c>
@@ -3585,7 +3596,8 @@
       </c>
       <c r="C13" s="33"/>
       <c r="D13" s="14">
-        <v>0</v>
+        <f>AVERAGE(D14:D17)</f>
+        <v>1</v>
       </c>
       <c r="E13" s="49">
         <v>45726</v>
@@ -3732,14 +3744,14 @@
       <c r="EJ13" s="22"/>
       <c r="EK13" s="22"/>
     </row>
-    <row r="14" spans="1:141" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:141" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="26"/>
       <c r="B14" s="40" t="s">
         <v>31</v>
       </c>
       <c r="C14" s="34"/>
       <c r="D14" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="51">
         <v>45726</v>
@@ -3886,14 +3898,14 @@
       <c r="EJ14" s="22"/>
       <c r="EK14" s="22"/>
     </row>
-    <row r="15" spans="1:141" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:141" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="25"/>
       <c r="B15" s="40" t="s">
         <v>32</v>
       </c>
       <c r="C15" s="34"/>
       <c r="D15" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="51">
         <v>45726</v>
@@ -4040,14 +4052,14 @@
       <c r="EJ15" s="22"/>
       <c r="EK15" s="22"/>
     </row>
-    <row r="16" spans="1:141" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:141" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="25"/>
       <c r="B16" s="40" t="s">
         <v>33</v>
       </c>
       <c r="C16" s="34"/>
       <c r="D16" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" s="51">
         <v>45726</v>
@@ -4194,14 +4206,14 @@
       <c r="EJ16" s="22"/>
       <c r="EK16" s="22"/>
     </row>
-    <row r="17" spans="1:141" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:141" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="25"/>
       <c r="B17" s="40" t="s">
         <v>34</v>
       </c>
       <c r="C17" s="34"/>
       <c r="D17" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" s="51">
         <v>45737</v>
@@ -4348,7 +4360,7 @@
       <c r="EJ17" s="22"/>
       <c r="EK17" s="22"/>
     </row>
-    <row r="18" spans="1:141" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:141" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="25" t="s">
         <v>11</v>
       </c>
@@ -4357,7 +4369,8 @@
       </c>
       <c r="C18" s="35"/>
       <c r="D18" s="17">
-        <v>0</v>
+        <f>AVERAGE(D19:D22)</f>
+        <v>0.1875</v>
       </c>
       <c r="E18" s="52">
         <v>45747</v>
@@ -4504,7 +4517,7 @@
       <c r="EJ18" s="22"/>
       <c r="EK18" s="22"/>
     </row>
-    <row r="19" spans="1:141" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:141" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="25"/>
       <c r="B19" s="41" t="s">
         <v>40</v>
@@ -4658,14 +4671,14 @@
       <c r="EJ19" s="22"/>
       <c r="EK19" s="22"/>
     </row>
-    <row r="20" spans="1:141" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:141" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="25"/>
       <c r="B20" s="41" t="s">
         <v>43</v>
       </c>
       <c r="C20" s="36"/>
       <c r="D20" s="18">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="E20" s="54">
         <v>45748</v>
@@ -4812,7 +4825,7 @@
       <c r="EJ20" s="22"/>
       <c r="EK20" s="22"/>
     </row>
-    <row r="21" spans="1:141" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:141" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="25"/>
       <c r="B21" s="41" t="s">
         <v>42</v>
@@ -4967,7 +4980,7 @@
       <c r="EJ21" s="22"/>
       <c r="EK21" s="22"/>
     </row>
-    <row r="22" spans="1:141" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:141" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="25"/>
       <c r="B22" s="41" t="s">
         <v>44</v>
@@ -5122,7 +5135,7 @@
       <c r="EJ22" s="22"/>
       <c r="EK22" s="22"/>
     </row>
-    <row r="23" spans="1:141" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:141" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="25" t="s">
         <v>11</v>
       </c>
@@ -5131,6 +5144,7 @@
       </c>
       <c r="C23" s="37"/>
       <c r="D23" s="20">
+        <f>AVERAGE(D24:D27)</f>
         <v>0</v>
       </c>
       <c r="E23" s="55">
@@ -5278,7 +5292,7 @@
       <c r="EJ23" s="22"/>
       <c r="EK23" s="22"/>
     </row>
-    <row r="24" spans="1:141" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:141" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="25"/>
       <c r="B24" s="42" t="s">
         <v>41</v>
@@ -5432,7 +5446,7 @@
       <c r="EJ24" s="22"/>
       <c r="EK24" s="22"/>
     </row>
-    <row r="25" spans="1:141" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:141" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="25"/>
       <c r="B25" s="42" t="s">
         <v>37</v>
@@ -5586,7 +5600,7 @@
       <c r="EJ25" s="22"/>
       <c r="EK25" s="22"/>
     </row>
-    <row r="26" spans="1:141" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:141" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="25"/>
       <c r="B26" s="42" t="s">
         <v>38</v>
@@ -5740,7 +5754,7 @@
       <c r="EJ26" s="22"/>
       <c r="EK26" s="22"/>
     </row>
-    <row r="27" spans="1:141" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:141" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="25"/>
       <c r="B27" s="42" t="s">
         <v>39</v>
@@ -5894,7 +5908,7 @@
       <c r="EJ27" s="22"/>
       <c r="EK27" s="22"/>
     </row>
-    <row r="28" spans="1:141" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:141" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="25" t="s">
         <v>11</v>
       </c>
@@ -5903,6 +5917,7 @@
       </c>
       <c r="C28" s="59"/>
       <c r="D28" s="60">
+        <f>AVERAGE(D29:D30)</f>
         <v>0</v>
       </c>
       <c r="E28" s="61">
@@ -6050,7 +6065,7 @@
       <c r="EJ28" s="22"/>
       <c r="EK28" s="22"/>
     </row>
-    <row r="29" spans="1:141" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:141" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="25"/>
       <c r="B29" s="63" t="s">
         <v>36</v>
@@ -6204,7 +6219,7 @@
       <c r="EJ29" s="22"/>
       <c r="EK29" s="22"/>
     </row>
-    <row r="30" spans="1:141" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:141" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="25"/>
       <c r="B30" s="63" t="s">
         <v>35</v>

</xml_diff>